<commit_message>
Updated as per the new data model (lower case)
</commit_message>
<xml_diff>
--- a/jcp-v2/60-rsconnectFiles/SKU_Div1-20Feb_Small_Match.xlsx
+++ b/jcp-v2/60-rsconnectFiles/SKU_Div1-20Feb_Small_Match.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
   <si>
     <t>10-SEP-15 11.58.06.607000000 AM</t>
   </si>
@@ -183,6 +183,33 @@
   </si>
   <si>
     <t>Violet</t>
+  </si>
+  <si>
+    <t>Hello2720010067</t>
+  </si>
+  <si>
+    <t>Hello2720010075</t>
+  </si>
+  <si>
+    <t>Hello2720010083</t>
+  </si>
+  <si>
+    <t>Hello2720010091</t>
+  </si>
+  <si>
+    <t>Hello2720010265</t>
+  </si>
+  <si>
+    <t>Hello2720010273</t>
+  </si>
+  <si>
+    <t>Hello2720010281</t>
+  </si>
+  <si>
+    <t>Hello2720010299</t>
+  </si>
+  <si>
+    <t>Hello2720010463</t>
   </si>
 </sst>
 </file>
@@ -542,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,8 +656,8 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>2720010067</v>
+      <c r="A2" t="s">
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -682,8 +709,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2720010075</v>
+      <c r="A3" t="s">
+        <v>54</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -735,8 +762,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2720010083</v>
+      <c r="A4" t="s">
+        <v>55</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -788,8 +815,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>2720010091</v>
+      <c r="A5" t="s">
+        <v>56</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -841,8 +868,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2720010265</v>
+      <c r="A6" t="s">
+        <v>57</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -894,8 +921,8 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>2720010273</v>
+      <c r="A7" t="s">
+        <v>58</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -947,8 +974,8 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>2720010281</v>
+      <c r="A8" t="s">
+        <v>59</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
@@ -1000,8 +1027,8 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>2720010299</v>
+      <c r="A9" t="s">
+        <v>60</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
@@ -1053,8 +1080,8 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>2720010463</v>
+      <c r="A10" t="s">
+        <v>61</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Corrected the mismatches in profile
</commit_message>
<xml_diff>
--- a/jcp-v2/60-rsconnectFiles/SKU_Div1-20Feb_Small_Match.xlsx
+++ b/jcp-v2/60-rsconnectFiles/SKU_Div1-20Feb_Small_Match.xlsx
@@ -185,31 +185,31 @@
     <t>Violet</t>
   </si>
   <si>
-    <t>Hello2720010067</t>
-  </si>
-  <si>
-    <t>Hello2720010075</t>
-  </si>
-  <si>
-    <t>Hello2720010083</t>
-  </si>
-  <si>
-    <t>Hello2720010091</t>
-  </si>
-  <si>
-    <t>Hello2720010265</t>
-  </si>
-  <si>
-    <t>Hello2720010273</t>
-  </si>
-  <si>
-    <t>Hello2720010281</t>
-  </si>
-  <si>
-    <t>Hello2720010299</t>
-  </si>
-  <si>
-    <t>Hello2720010463</t>
+    <t>World2720010067</t>
+  </si>
+  <si>
+    <t>World2720010075</t>
+  </si>
+  <si>
+    <t>World2720010083</t>
+  </si>
+  <si>
+    <t>World2720010091</t>
+  </si>
+  <si>
+    <t>World2720010265</t>
+  </si>
+  <si>
+    <t>World2720010273</t>
+  </si>
+  <si>
+    <t>World2720010281</t>
+  </si>
+  <si>
+    <t>World2720010299</t>
+  </si>
+  <si>
+    <t>World2720010463</t>
   </si>
 </sst>
 </file>
@@ -570,7 +570,7 @@
   <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>